<commit_message>
updated electrode definition template excel table to include planning length and specific depth electrode types
</commit_message>
<xml_diff>
--- a/Tools/ElectrodeDefinitionTemplate/ElectrodeDefinitionTemplate.xlsx
+++ b/Tools/ElectrodeDefinitionTemplate/ElectrodeDefinitionTemplate.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29525"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamesswift/Documents/git/VERA/Tools/ElectrodeDefinitionTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6FB20C5-7647-2143-8DE7-3B418AF53C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2AD5A705-AFEC-4DA6-A51C-C67CFBF8E206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="7940" windowWidth="38680" windowHeight="17440" xr2:uid="{53C836AE-3208-234C-832C-600E8D41075E}"/>
+    <workbookView xWindow="4360" yWindow="7940" windowWidth="38680" windowHeight="17440" activeTab="1" xr2:uid="{53C836AE-3208-234C-832C-600E8D41075E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Type</t>
   </si>
@@ -45,27 +45,48 @@
     <t>Name</t>
   </si>
   <si>
+    <t>NElectrodes</t>
+  </si>
+  <si>
+    <t>Spacing</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>PlanningLength</t>
+  </si>
+  <si>
+    <t>Depth</t>
+  </si>
+  <si>
     <t>Nelectrodes</t>
   </si>
   <si>
-    <t>Spacing</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
-    <t>Depth</t>
-  </si>
-  <si>
     <t>Micro</t>
   </si>
   <si>
     <t>Grid</t>
   </si>
   <si>
+    <t>Strip (Projectable)</t>
+  </si>
+  <si>
     <t>Strip</t>
   </si>
   <si>
+    <t>Depth (DIXI)</t>
+  </si>
+  <si>
+    <t>Depth (Adtech)</t>
+  </si>
+  <si>
+    <t>Depth (PMT)</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
     <t>DBS</t>
   </si>
   <si>
@@ -76,22 +97,13 @@
   </si>
   <si>
     <t>Boston Vercise Directional</t>
-  </si>
-  <si>
-    <t>NElectrodes</t>
-  </si>
-  <si>
-    <t>GND</t>
-  </si>
-  <si>
-    <t>Strip (Projectable)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -456,15 +468,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9B4950-0C02-D049-9B8B-9EBECAEE451E}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
+  <cols>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -472,13 +487,21 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -488,7 +511,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{87F7CC15-E5D7-F149-945B-C59AAB6D7A17}">
           <x14:formula1>
-            <xm:f>Sheet2!$A$2:$A$11</xm:f>
+            <xm:f>Sheet2!$A$2:$A$14</xm:f>
           </x14:formula1>
           <xm:sqref>A2</xm:sqref>
         </x14:dataValidation>
@@ -500,18 +523,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BA9FDD-1A88-F94F-867C-1AEE5E9AE967}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
+    <col min="1" max="1" width="22.625" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -519,7 +543,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -527,55 +551,73 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:6" ht="15.75">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>